<commit_message>
Fixing issues with jobs option.
</commit_message>
<xml_diff>
--- a/Data/Input/InputFile.xlsx
+++ b/Data/Input/InputFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ProyectosPortafolio\RoboticEnterpriseFramework\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ProyectosPortafolio\LInkedIn\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F850333C-7FC1-4AE6-9B95-E092ACF030AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0230A8A-8D9F-4DAE-9B9D-234188D51765}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9804" xr2:uid="{4A5DAAA0-D581-479D-9886-92F8A279D228}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Type</t>
   </si>
@@ -43,13 +43,7 @@
     <t>People</t>
   </si>
   <si>
-    <t>HR Recutrier</t>
-  </si>
-  <si>
     <t>Developer</t>
-  </si>
-  <si>
-    <t>Junior Dev React</t>
   </si>
   <si>
     <t>City</t>
@@ -138,8 +132,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D085422-AFF2-4AC6-8E38-2E836FAB4322}" name="Tabla2" displayName="Tabla2" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{52F5CE92-1ED3-44BB-AE59-AB72762E1309}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D085422-AFF2-4AC6-8E38-2E836FAB4322}" name="Tabla2" displayName="Tabla2" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{52F5CE92-1ED3-44BB-AE59-AB72762E1309}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E16E2865-1D10-4495-9986-6E885D69856F}" name="Type"/>
     <tableColumn id="2" xr3:uid="{304F5ADE-75FA-405D-BC46-29B322B1B0F6}" name="KeyWords"/>
@@ -447,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E47D87C-3858-4CA2-8377-DC8874FF0514}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,21 +461,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -489,22 +483,14 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -518,7 +504,7 @@
           <x14:formula1>
             <xm:f>Valores!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A4</xm:sqref>
+          <xm:sqref>A2:A3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fixed issue with time to wait for the page to load.
</commit_message>
<xml_diff>
--- a/Data/Input/InputFile.xlsx
+++ b/Data/Input/InputFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ProyectosPortafolio\LInkedIn\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0230A8A-8D9F-4DAE-9B9D-234188D51765}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F08A33-87B0-4E15-B7DF-8DBCDCC200AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9804" xr2:uid="{4A5DAAA0-D581-479D-9886-92F8A279D228}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +478,7 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>